<commit_message>
Update projects dan publications
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aldilasan/Documents/Github/cv-aldilas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D3B934-14D4-4102-BA99-FF616E2959DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3752A9-B2D1-064A-9835-7A35F8E867C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{481E0DEE-DD0F-456B-BB19-2C6D312E1D40}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{481E0DEE-DD0F-456B-BB19-2C6D312E1D40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Period</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>Consultant : Conducting Post-Abortion Care Supply Chain Management assesment in Indonesia involving MoH, public health office staffs, public health center staffs, hospital staffs, and post-abortion care logistics supplier.; Responsible for designing methodology and instruments.; Responsible for data quantitative and qualitative data collection and analysis.</t>
+  </si>
+  <si>
+    <t>2021-2022</t>
+  </si>
+  <si>
+    <t>2021-present</t>
   </si>
 </sst>
 </file>
@@ -483,17 +489,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C9E173-AAE7-4932-87DD-E12026BA5502}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,29 +510,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>2021</v>
+    <row r="2" spans="1:3" ht="256" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="300" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2021</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2020</v>
       </c>
@@ -537,7 +543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2020</v>
       </c>
@@ -548,7 +554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2019</v>
       </c>
@@ -559,7 +565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>